<commit_message>
Adding some corrections as well as emptying the charts in the word document
</commit_message>
<xml_diff>
--- a/11_heart_failure/11_heart_failure_data.xlsx
+++ b/11_heart_failure/11_heart_failure_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="21075" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20730" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Heart Failure Data</t>
   </si>
@@ -232,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -249,22 +249,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -563,7 +566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
       <selection activeCell="G7" sqref="G7:H8"/>
     </sheetView>
   </sheetViews>
@@ -578,7 +581,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -593,30 +596,30 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="M2" s="9" t="s">
+      <c r="M2" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A3" s="7"/>
+      <c r="A3" s="12"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -629,7 +632,7 @@
       <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="3">
@@ -667,25 +670,25 @@
       <c r="E4" s="5">
         <v>86</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>0</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>0</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>0.02</v>
       </c>
-      <c r="K4" s="10">
+      <c r="K4" s="9">
         <v>0.04</v>
       </c>
-      <c r="L4" s="10">
+      <c r="L4" s="9">
         <v>0.06</v>
       </c>
-      <c r="M4" s="10">
+      <c r="M4" s="9">
         <v>0.08</v>
       </c>
     </row>
@@ -705,11 +708,11 @@
       <c r="E5" s="5">
         <v>4907</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="6" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="5">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="I5" s="5">
         <v>126</v>
@@ -718,10 +721,10 @@
         <v>137</v>
       </c>
       <c r="K5" s="5">
-        <v>149</v>
-      </c>
-      <c r="L5" s="5">
-        <v>176</v>
+        <v>148</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>30</v>
@@ -763,8 +766,8 @@
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="11">
-        <v>0.19583333333333333</v>
+      <c r="H7" s="10">
+        <v>0.15416666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60.75" thickBot="1">
@@ -786,8 +789,8 @@
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="8">
-        <v>1953</v>
+      <c r="H8" s="7">
+        <v>1957</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" thickBot="1">
@@ -842,52 +845,52 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="11">
         <v>2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="11">
         <v>2</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="11">
         <v>1.8</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="11">
         <v>0.12</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="11">
         <v>0.08</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="11">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="11">
         <v>0.13</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
     </row>
     <row r="16" spans="1:13" ht="45.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -976,17 +979,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding labs 11 and 13
</commit_message>
<xml_diff>
--- a/11_heart_failure/11_heart_failure_data.xlsx
+++ b/11_heart_failure/11_heart_failure_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>Heart Failure Data</t>
   </si>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G7" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:H8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -659,10 +659,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="5">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D4" s="5">
         <v>84</v>
@@ -697,16 +697,16 @@
         <v>6</v>
       </c>
       <c r="B5" s="5">
-        <v>5361</v>
+        <v>5346</v>
       </c>
       <c r="C5" s="5">
-        <v>4757</v>
+        <v>4777</v>
       </c>
       <c r="D5" s="5">
-        <v>4649</v>
+        <v>4597</v>
       </c>
       <c r="E5" s="5">
-        <v>4907</v>
+        <v>4607</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>29</v>
@@ -715,16 +715,16 @@
         <v>70</v>
       </c>
       <c r="I5" s="5">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J5" s="5">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K5" s="5">
-        <v>148</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>30</v>
+        <v>146</v>
+      </c>
+      <c r="L5" s="5">
+        <v>182</v>
       </c>
       <c r="M5" s="5" t="s">
         <v>30</v>
@@ -738,10 +738,10 @@
         <v>72</v>
       </c>
       <c r="C6" s="5">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="5">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6" s="5">
         <v>70</v>
@@ -752,22 +752,22 @@
         <v>8</v>
       </c>
       <c r="B7" s="5">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="5">
         <v>64</v>
       </c>
       <c r="D7" s="5">
+        <v>65</v>
+      </c>
+      <c r="E7" s="5">
         <v>66</v>
-      </c>
-      <c r="E7" s="5">
-        <v>70</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="10">
-        <v>0.15416666666666667</v>
+        <v>0.1673611111111111</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60.75" thickBot="1">
@@ -778,19 +778,19 @@
         <v>124</v>
       </c>
       <c r="C8" s="5">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" s="5">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E8" s="5">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="7">
-        <v>1957</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" thickBot="1">
@@ -798,16 +798,16 @@
         <v>10</v>
       </c>
       <c r="B9" s="5">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="C9" s="5">
-        <v>8.4</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5">
-        <v>8.6</v>
+        <v>7.9</v>
       </c>
       <c r="E9" s="5">
-        <v>7.8</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60.75" thickBot="1">
@@ -818,13 +818,13 @@
         <v>0.6</v>
       </c>
       <c r="C10" s="5">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="D10" s="5">
         <v>0.43</v>
       </c>
       <c r="E10" s="5">
-        <v>0.47</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45.75" thickBot="1">
@@ -855,10 +855,10 @@
         <v>2</v>
       </c>
       <c r="D12" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="E12" s="11">
         <v>2.2000000000000002</v>
-      </c>
-      <c r="E12" s="11">
-        <v>1.8</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
@@ -876,13 +876,13 @@
         <v>0.12</v>
       </c>
       <c r="C14" s="11">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="D14" s="11">
-        <v>7.0000000000000007E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E14" s="11">
-        <v>0.13</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1">
@@ -897,16 +897,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5">
+        <v>12</v>
+      </c>
+      <c r="E16" s="5">
         <v>8</v>
-      </c>
-      <c r="E16" s="5">
-        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45.75" thickBot="1">
@@ -914,16 +914,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="5">
-        <v>5400</v>
+        <v>5413</v>
       </c>
       <c r="C17" s="5">
-        <v>5399</v>
+        <v>5409</v>
       </c>
       <c r="D17" s="5">
-        <v>5450</v>
+        <v>5408</v>
       </c>
       <c r="E17" s="5">
-        <v>5491</v>
+        <v>5396</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60.75" thickBot="1">
@@ -931,16 +931,16 @@
         <v>17</v>
       </c>
       <c r="B18" s="5">
-        <v>2400</v>
+        <v>2451</v>
       </c>
       <c r="C18" s="5">
-        <v>2400</v>
+        <v>2451</v>
       </c>
       <c r="D18" s="5">
-        <v>2399</v>
+        <v>2451</v>
       </c>
       <c r="E18" s="5">
-        <v>2367</v>
+        <v>2421</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="45.75" thickBot="1">
@@ -948,16 +948,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="5">
-        <v>3000</v>
+        <v>2962</v>
       </c>
       <c r="C19" s="5">
-        <v>2999</v>
+        <v>2958</v>
       </c>
       <c r="D19" s="5">
-        <v>3052</v>
+        <v>2958</v>
       </c>
       <c r="E19" s="5">
-        <v>3124</v>
+        <v>2976</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="30.75" thickBot="1">
@@ -965,31 +965,31 @@
         <v>19</v>
       </c>
       <c r="B20" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D20" s="5">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E20" s="5">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding labs 13 and 11
</commit_message>
<xml_diff>
--- a/11_heart_failure/11_heart_failure_data.xlsx
+++ b/11_heart_failure/11_heart_failure_data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>Heart Failure Data</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Distance Traveled (Ft)</t>
+  </si>
+  <si>
+    <t>QCP</t>
+  </si>
+  <si>
+    <t>HumMod</t>
   </si>
 </sst>
 </file>
@@ -232,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -264,10 +270,16 @@
     <xf numFmtId="20" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -576,12 +588,15 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>33</v>
+      </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -619,7 +634,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A3" s="12"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -845,52 +860,52 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="12">
         <v>2</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="12">
         <v>2</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="12">
         <v>2.5</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="12">
         <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="44.25" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="12">
         <v>0.12</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="12">
         <v>0.09</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="12">
         <v>0.04</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="12">
         <v>0.11</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" thickBot="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="45.75" thickBot="1">
       <c r="A16" s="4" t="s">
@@ -909,7 +924,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="45.75" thickBot="1">
+    <row r="17" spans="1:13" ht="45.75" thickBot="1">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -926,7 +941,7 @@
         <v>5396</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60.75" thickBot="1">
+    <row r="18" spans="1:13" ht="60.75" thickBot="1">
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
@@ -943,7 +958,7 @@
         <v>2421</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="45.75" thickBot="1">
+    <row r="19" spans="1:13" ht="45.75" thickBot="1">
       <c r="A19" s="4" t="s">
         <v>18</v>
       </c>
@@ -960,7 +975,7 @@
         <v>2976</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30.75" thickBot="1">
+    <row r="20" spans="1:13" ht="30.75" thickBot="1">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
@@ -977,19 +992,432 @@
         <v>45</v>
       </c>
     </row>
+    <row r="23" spans="1:13" ht="30.75" thickBot="1">
+      <c r="A23" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A24" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M24" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1">
+      <c r="A25" s="13"/>
+      <c r="B25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H25" s="3">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <v>6</v>
+      </c>
+      <c r="J25" s="3">
+        <v>6</v>
+      </c>
+      <c r="K25" s="3">
+        <v>6</v>
+      </c>
+      <c r="L25" s="3">
+        <v>6</v>
+      </c>
+      <c r="M25" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A26" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="5">
+        <v>96.6</v>
+      </c>
+      <c r="C26" s="5">
+        <v>96.9</v>
+      </c>
+      <c r="D26" s="5">
+        <v>97</v>
+      </c>
+      <c r="E26" s="5">
+        <v>96.9</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0.06</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="75.75" thickBot="1">
+      <c r="A27" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="5">
+        <v>5468</v>
+      </c>
+      <c r="C27" s="5">
+        <v>5442</v>
+      </c>
+      <c r="D27" s="5">
+        <v>5448</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5433</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="5">
+        <v>80</v>
+      </c>
+      <c r="I27" s="5">
+        <v>139</v>
+      </c>
+      <c r="J27" s="5">
+        <v>146</v>
+      </c>
+      <c r="K27" s="5">
+        <v>149</v>
+      </c>
+      <c r="L27" s="5">
+        <v>161</v>
+      </c>
+      <c r="M27" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A28" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5">
+        <v>72</v>
+      </c>
+      <c r="C28" s="5">
+        <v>72</v>
+      </c>
+      <c r="D28" s="5">
+        <v>72</v>
+      </c>
+      <c r="E28" s="5">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A29" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="5">
+        <v>76</v>
+      </c>
+      <c r="C29" s="5">
+        <v>76</v>
+      </c>
+      <c r="D29" s="5">
+        <v>76</v>
+      </c>
+      <c r="E29" s="5">
+        <v>75</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0.20416666666666669</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="5">
+        <v>126.7</v>
+      </c>
+      <c r="C30" s="5">
+        <v>126.7</v>
+      </c>
+      <c r="D30" s="5">
+        <v>126.7</v>
+      </c>
+      <c r="E30" s="5">
+        <v>126.3</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="7">
+        <v>2588</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="45.75" thickBot="1">
+      <c r="A31" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="C31" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="D31" s="5">
+        <v>5.2</v>
+      </c>
+      <c r="E31" s="5">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="60.75" thickBot="1">
+      <c r="A32" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="D32" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="E32" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="C33" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E33" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="60.75" thickBot="1">
+      <c r="A34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C34" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D34" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E34" s="5">
+        <v>2.2999999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="44.25" customHeight="1">
+      <c r="A35" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="12">
+        <v>0.123</v>
+      </c>
+      <c r="C35" s="12">
+        <v>0.125</v>
+      </c>
+      <c r="D35" s="12">
+        <v>0.126</v>
+      </c>
+      <c r="E35" s="12">
+        <v>0.123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+    </row>
+    <row r="37" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A37" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="C37" s="5">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="D37" s="5">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="E37" s="5">
+        <v>19.100000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A38" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5421</v>
+      </c>
+      <c r="C38" s="5">
+        <v>5421</v>
+      </c>
+      <c r="D38" s="5">
+        <v>5412</v>
+      </c>
+      <c r="E38" s="5">
+        <v>5400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="44.25" customHeight="1">
+      <c r="A39" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="12">
+        <v>2340</v>
+      </c>
+      <c r="C39" s="12">
+        <v>2430</v>
+      </c>
+      <c r="D39" s="12">
+        <v>2340</v>
+      </c>
+      <c r="E39" s="12">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+    </row>
+    <row r="41" spans="1:5" ht="45.75" thickBot="1">
+      <c r="A41" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="5">
+        <v>3081</v>
+      </c>
+      <c r="C41" s="5">
+        <v>3080</v>
+      </c>
+      <c r="D41" s="5">
+        <v>3071</v>
+      </c>
+      <c r="E41" s="5">
+        <v>3058</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="30.75" thickBot="1">
+      <c r="A42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="5">
+        <v>43</v>
+      </c>
+      <c r="C42" s="5">
+        <v>43</v>
+      </c>
+      <c r="D42" s="5">
+        <v>43</v>
+      </c>
+      <c r="E42" s="5">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
+  <mergeCells count="22">
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>